<commit_message>
Added classes and refactor superjob
</commit_message>
<xml_diff>
--- a/lession2/task1/output.xlsx
+++ b/lession2/task1/output.xlsx
@@ -399,20 +399,24 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Инженер-программист группы разработки ПО</t>
+          <t>Пекарь (м. Арбатская)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-gruppy-razrabotki-po-32499770.html</t>
+          <t>http://www.superjob.ru/vakansii/pekar-32268014.html</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>100000</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -425,12 +429,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Контролер на склад товаров для магазина</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32227306.html</t>
+          <t>http://www.superjob.ru/vakansii/kontroler-na-sklad-tovarov-dlya-magazina-32335576.html</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -451,17 +455,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Визитный мерчендайзер</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32257674.html</t>
+          <t>http://www.superjob.ru/vakansii/vizitnyj-merchendajzer-32335578.html</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>3900</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -477,12 +481,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Оператор по работе с клиентами</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32132422.html</t>
+          <t>http://www.superjob.ru/vakansii/operator-po-rabote-s-klientami-32292362.html</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -503,17 +507,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Программист-консультант 1С</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-konsultant-1s-32462380.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32292911.html</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>30000</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -529,22 +533,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ведущий программист мобильных приложений на 1С</t>
+          <t>Продавец-консультант (м. Новокосино, Новогиреево)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/vakansii/veduschij-programmist-mobilnyh-prilozhenij-na-1s-32445138.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32392050.html</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>184000</t>
+          <t>45000</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>212000</t>
+          <t>51000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -559,20 +563,24 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Программист в единственном лице на производство</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-v-edinstvennom-lice-na-proizvodstvo-32526399.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-31806604.html</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>150000</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>95000</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -585,17 +593,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Старший повар</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32431672.html</t>
+          <t>http://www.superjob.ru/vakansii/starshij-povar-32292909.html</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>35000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -611,17 +619,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Директор магазина</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-31216750.html</t>
+          <t>http://www.superjob.ru/vakansii/direktor-magazina-32240008.html</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>100000</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -637,20 +645,24 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Педагог-психолог</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32271142.html</t>
+          <t>http://www.superjob.ru/vakansii/pedagog-psiholog-32116732.html</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>120000</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>48000</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -663,17 +675,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Водитель такси категории Б</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-29393223.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-taksi-kategorii-b-32454117.html</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>150000</t>
+          <t>Не указано</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -689,24 +701,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Программист С++, Golang, PHP, Python, DevOPS (релокация на о. Бали)</t>
+          <t>Медицинская сестра отделения вспомогательных репродуктивных технологий</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-s-32517185.html</t>
+          <t>http://www.superjob.ru/vakansii/medicinskaya-sestra-otdeleniya-vspomogatelnyh-reproduktivnyh-tehnologij-32434455.html</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>100000</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>250000</t>
-        </is>
-      </c>
+          <t>Не указано</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -719,20 +727,24 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Электронщик-программист ПЛК</t>
+          <t>Продавец-консультант (ст. м. Фили)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>/vakansii/elektronschik-programmist-plk-31976254.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-29970309.html</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>58000</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>78000</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -745,12 +757,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Водитель на минивэн</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32363006.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-na-miniven-30987950.html</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -771,17 +783,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Начинающий специалист по обслуживанию клиентов</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32525359.html</t>
+          <t>http://www.superjob.ru/vakansii/nachinayuschij-specialist-po-obsluzhivaniyu-klientov-31670219.html</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>40000</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -797,20 +809,24 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Программист PHP</t>
+          <t>Повар (м. Фрунзенская)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-php-32039622.html</t>
+          <t>http://www.superjob.ru/vakansii/povar-32268013.html</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -823,17 +839,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Продавец в супермаркет премиум-класса (Истринскй р-н, д. Покровское)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32430883.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-v-supermarket-premium-klassa-31128173.html</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>43000</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -849,17 +865,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Инженер-программист C++</t>
+          <t>Менеджер в минимаркет премиум-класса (м. Беговая, Университет, Выставочная, Деловой центр)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-c-31999834.html</t>
+          <t>http://www.superjob.ru/vakansii/menedzher-v-minimarket-premium-klassa-31160269.html</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>47850</t>
+          <t>45000</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -875,12 +891,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Программист Android 4.2 (технологии DI, SQLite)</t>
+          <t>Мастер участка по ремонту кабельных линий 14 РЭР</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-android-4-32327168.html</t>
+          <t>http://www.superjob.ru/vakansii/master-uchastka-po-remontu-kabelnyh-linij-14-rer-32330202.html</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -901,17 +917,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Программист SQL</t>
+          <t>Риелтор по недвижимости</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-sql-30873935.html</t>
+          <t>http://www.superjob.ru/vakansii/rieltor-po-nedvizhimosti-32379651.html</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>90000</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -927,20 +943,24 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Инженер-программист</t>
+          <t>Пекарь (м. Арбатская)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-32407139.html</t>
+          <t>http://www.superjob.ru/vakansii/pekar-32268014.html</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>80000</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -953,17 +973,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Инженер-программист</t>
+          <t>Контролер на склад товаров для магазина</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-32227325.html</t>
+          <t>http://www.superjob.ru/vakansii/kontroler-na-sklad-tovarov-dlya-magazina-32335576.html</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>120000</t>
+          <t>Не указано</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -979,17 +999,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Программист C++</t>
+          <t>Визитный мерчендайзер</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-c-32401530.html</t>
+          <t>http://www.superjob.ru/vakansii/vizitnyj-merchendajzer-32335578.html</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>3900</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -1005,17 +1025,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Программист 1С (CRM)</t>
+          <t>Оператор по работе с клиентами</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-31989158.html</t>
+          <t>http://www.superjob.ru/vakansii/operator-po-rabote-s-klientami-32292362.html</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>130000</t>
+          <t>Не указано</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1031,17 +1051,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32122929.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32292911.html</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>30000</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1057,20 +1077,24 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Программист / Разработчик</t>
+          <t>Продавец-консультант (м. Новокосино, Новогиреево)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-32274027.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32392050.html</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>51000</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1083,22 +1107,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Программист Delphi</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-delphi-30280217.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-31806604.html</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>100000</t>
+          <t>45000</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>120000</t>
+          <t>95000</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1113,17 +1137,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Программист ЛИМС-интеграции</t>
+          <t>Старший повар</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-lims-integracii-32013112.html</t>
+          <t>http://www.superjob.ru/vakansii/starshij-povar-32292909.html</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>70000</t>
+          <t>35000</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1139,24 +1163,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Программист java (стажер)</t>
+          <t>Директор магазина</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-java-29932190.html</t>
+          <t>http://www.superjob.ru/vakansii/direktor-magazina-32240008.html</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>50000</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>60000</t>
-        </is>
-      </c>
+          <t>80000</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1169,20 +1189,24 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Программист javascript (телекоммуникационные услуги связи)</t>
+          <t>Педагог-психолог</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-javascript-32159051.html</t>
+          <t>http://www.superjob.ru/vakansii/pedagog-psiholog-32116732.html</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>60000</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>48000</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1195,12 +1219,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Водитель такси категории Б</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-31703659.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-taksi-kategorii-b-32454117.html</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1221,12 +1245,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Программист Android (Kotlin)</t>
+          <t>Медицинская сестра отделения вспомогательных репродуктивных технологий</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-android-32429207.html</t>
+          <t>http://www.superjob.ru/vakansii/medicinskaya-sestra-otdeleniya-vspomogatelnyh-reproduktivnyh-tehnologij-32434455.html</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1247,20 +1271,24 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Продавец-консультант (ст. м. Фили)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-31830483.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-29970309.html</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>58000</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>78000</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1273,12 +1301,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Водитель на минивэн</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32502911.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-na-miniven-30987950.html</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1299,24 +1327,20 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Программист 1С (удаленная работа)</t>
+          <t>Начинающий специалист по обслуживанию клиентов</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-30967007.html</t>
+          <t>http://www.superjob.ru/vakansii/nachinayuschij-specialist-po-obsluzhivaniyu-klientov-31670219.html</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>90000</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>120000</t>
-        </is>
-      </c>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1329,20 +1353,24 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Ведущий инженер-программист</t>
+          <t>Повар (м. Фрунзенская)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>/vakansii/veduschij-inzhener-programmist-31760440.html</t>
+          <t>http://www.superjob.ru/vakansii/povar-32268013.html</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>100000</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1355,17 +1383,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Программист микроконтроллеров С/С++</t>
+          <t>Продавец в супермаркет премиум-класса (Истринскй р-н, д. Покровское)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-mikrokontrollerov-s-32489761.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-v-supermarket-premium-klassa-31128173.html</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>43000</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1381,24 +1409,20 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Менеджер в минимаркет премиум-класса (м. Беговая, Университет, Выставочная, Деловой центр)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-30753446.html</t>
+          <t>http://www.superjob.ru/vakansii/menedzher-v-minimarket-premium-klassa-31160269.html</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>50000</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>200000</t>
-        </is>
-      </c>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1411,24 +1435,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Программист 1С Bitrix</t>
+          <t>Мастер участка по ремонту кабельных линий 14 РЭР</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-bitrix-31388659.html</t>
+          <t>http://www.superjob.ru/vakansii/master-uchastka-po-remontu-kabelnyh-linij-14-rer-32330202.html</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>50000</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>150000</t>
-        </is>
-      </c>
+          <t>Не указано</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1441,17 +1461,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Разработчик / Программист / Developer (Angular 2+) (Junior, Middle, Senior)</t>
+          <t>Риелтор по недвижимости</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>/vakansii/razrabotchik-31734252.html</t>
+          <t>http://www.superjob.ru/vakansii/rieltor-po-nedvizhimosti-32379651.html</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -1467,20 +1487,24 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Программист встраиваемых систем, инженер-схемотехник</t>
+          <t>Пекарь (м. Арбатская)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-vstraivaemyh-sistem-32522553.html</t>
+          <t>http://www.superjob.ru/vakansii/pekar-32268014.html</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>80000</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1493,24 +1517,20 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Контролер на склад товаров для магазина</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32174069.html</t>
+          <t>http://www.superjob.ru/vakansii/kontroler-na-sklad-tovarov-dlya-magazina-32335576.html</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>100000</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>170000</t>
-        </is>
-      </c>
+          <t>Не указано</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1523,24 +1543,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Администратор сайта на Bitrix, программист</t>
+          <t>Визитный мерчендайзер</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>/vakansii/administrator-sajta-na-bitrix-32360782.html</t>
+          <t>http://www.superjob.ru/vakansii/vizitnyj-merchendajzer-32335578.html</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>50000</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>70000</t>
-        </is>
-      </c>
+          <t>3900</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1553,17 +1569,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Оператор / Наладчик / Программист станка с ЧПУ</t>
+          <t>Оператор по работе с клиентами</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>/vakansii/operator-11424776.html</t>
+          <t>http://www.superjob.ru/vakansii/operator-po-rabote-s-klientami-32292362.html</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>100000</t>
+          <t>Не указано</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1579,24 +1595,20 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Web-программист / Web-разработчик</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>/vakansii/web-programmist-29723693.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32292911.html</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>150000</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>200000</t>
-        </is>
-      </c>
+          <t>30000</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1609,20 +1621,24 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Ведущий программист 1С 8</t>
+          <t>Продавец-консультант (м. Новокосино, Новогиреево)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>/vakansii/veduschij-programmist-1s-8-32399181.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32392050.html</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>150000</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>51000</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1635,20 +1651,24 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-30708588.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-31806604.html</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>95000</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1661,17 +1681,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Ведущий программист 1С</t>
+          <t>Старший повар</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>/vakansii/veduschij-programmist-1s-31746539.html</t>
+          <t>http://www.superjob.ru/vakansii/starshij-povar-32292909.html</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>35000</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -1687,12 +1707,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Программист C++ Builder</t>
+          <t>Директор магазина</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-c-32440680.html</t>
+          <t>http://www.superjob.ru/vakansii/direktor-magazina-32240008.html</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1713,20 +1733,24 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Педагог-психолог</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32464172.html</t>
+          <t>http://www.superjob.ru/vakansii/pedagog-psiholog-32116732.html</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>160000</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr"/>
+          <t>48000</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1739,24 +1763,20 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Инженер-программист ЧПУ</t>
+          <t>Водитель такси категории Б</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-chpu-32457401.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-taksi-kategorii-b-32454117.html</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>70000</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>130000</t>
-        </is>
-      </c>
+          <t>Не указано</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1769,12 +1789,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Медицинская сестра отделения вспомогательных репродуктивных технологий</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32373763.html</t>
+          <t>http://www.superjob.ru/vakansii/medicinskaya-sestra-otdeleniya-vspomogatelnyh-reproduktivnyh-tehnologij-32434455.html</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1795,22 +1815,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Программист</t>
+          <t>Продавец-консультант (ст. м. Фили)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-32427127.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-29970309.html</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>50000</t>
+          <t>58000</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>80000</t>
+          <t>78000</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -1825,17 +1845,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Программист C#</t>
+          <t>Водитель на минивэн</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-c-30558941.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-na-miniven-30987950.html</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>160000</t>
+          <t>100000</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -1851,24 +1871,20 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Программист</t>
+          <t>Начинающий специалист по обслуживанию клиентов</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-30736873.html</t>
+          <t>http://www.superjob.ru/vakansii/nachinayuschij-specialist-po-obsluzhivaniyu-klientov-31670219.html</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>30000</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>60000</t>
-        </is>
-      </c>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1881,20 +1897,24 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Программист станков с ЧПУ / Технолог-программист / Инженер-технолог по механообработке</t>
+          <t>Повар (м. Фрунзенская)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-stankov-s-chpu-32514664.html</t>
+          <t>http://www.superjob.ru/vakansii/povar-32268013.html</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1907,17 +1927,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Программист НТЦ</t>
+          <t>Продавец в супермаркет премиум-класса (Истринскй р-н, д. Покровское)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-ntc-32514641.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-v-supermarket-premium-klassa-31128173.html</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>43000</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -1933,17 +1953,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Менеджер в минимаркет премиум-класса (м. Беговая, Университет, Выставочная, Деловой центр)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32493217.html</t>
+          <t>http://www.superjob.ru/vakansii/menedzher-v-minimarket-premium-klassa-31160269.html</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>45000</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -1959,24 +1979,20 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Программист Visual Basic</t>
+          <t>Мастер участка по ремонту кабельных линий 14 РЭР</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-visual-basic-32261511.html</t>
+          <t>http://www.superjob.ru/vakansii/master-uchastka-po-remontu-kabelnyh-linij-14-rer-32330202.html</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>50000</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>80000</t>
-        </is>
-      </c>
+          <t>Не указано</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -1989,17 +2005,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Риелтор по недвижимости</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-31043425.html</t>
+          <t>http://www.superjob.ru/vakansii/rieltor-po-nedvizhimosti-32379651.html</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -2015,20 +2031,24 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Ведущий инженер-программист веб-интерфейсов (Frontend Angular)</t>
+          <t>Пекарь (м. Арбатская)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>/vakansii/veduschij-inzhener-programmist-veb-interfejsov-32514347.html</t>
+          <t>http://www.superjob.ru/vakansii/pekar-32268014.html</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>170000</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2041,12 +2061,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Контролер на склад товаров для магазина</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32469438.html</t>
+          <t>http://www.superjob.ru/vakansii/kontroler-na-sklad-tovarov-dlya-magazina-32335576.html</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2067,24 +2087,20 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Программист 1С, системный администратор, маркетолог</t>
+          <t>Визитный мерчендайзер</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-30509816.html</t>
+          <t>http://www.superjob.ru/vakansii/vizitnyj-merchendajzer-32335578.html</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>50000</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>65000</t>
-        </is>
-      </c>
+          <t>3900</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2097,12 +2113,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Помощник программиста 1С</t>
+          <t>Оператор по работе с клиентами</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>/vakansii/pomoschnik-programmista-1s-31819093.html</t>
+          <t>http://www.superjob.ru/vakansii/operator-po-rabote-s-klientami-32292362.html</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2123,17 +2139,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Программист контроллеров</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-kontrollerov-32041389.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32292911.html</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>50000</t>
+          <t>30000</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -2149,20 +2165,24 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Продавец-консультант (м. Новокосино, Новогиреево)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-31844442.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32392050.html</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>51000</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2175,20 +2195,24 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Программист базы данных</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-bazy-dannyh-32397479.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-31806604.html</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr"/>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>95000</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2201,24 +2225,20 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Программист 1С 8</t>
+          <t>Старший повар</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-8-31698967.html</t>
+          <t>http://www.superjob.ru/vakansii/starshij-povar-32292909.html</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>130000</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>150000</t>
-        </is>
-      </c>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2231,17 +2251,17 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Программист SQL</t>
+          <t>Директор магазина</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-sql-30790592.html</t>
+          <t>http://www.superjob.ru/vakansii/direktor-magazina-32240008.html</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
@@ -2257,20 +2277,24 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Педагог-психолог</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32002546.html</t>
+          <t>http://www.superjob.ru/vakansii/pedagog-psiholog-32116732.html</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr"/>
+          <t>48000</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
       <c r="F71" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2283,24 +2307,20 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Инженер-программист</t>
+          <t>Водитель такси категории Б</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-32397220.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-taksi-kategorii-b-32454117.html</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>75000</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>85000</t>
-        </is>
-      </c>
+          <t>Не указано</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2313,24 +2333,20 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Ведущий инженер-программист C/C++</t>
+          <t>Медицинская сестра отделения вспомогательных репродуктивных технологий</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>/vakansii/veduschij-inzhener-programmist-c-31456745.html</t>
+          <t>http://www.superjob.ru/vakansii/medicinskaya-sestra-otdeleniya-vspomogatelnyh-reproduktivnyh-tehnologij-32434455.html</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>85000</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>95000</t>
-        </is>
-      </c>
+          <t>Не указано</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2343,20 +2359,24 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Программист Битрикс</t>
+          <t>Продавец-консультант (ст. м. Фили)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-bitriks-32425390.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-29970309.html</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr"/>
+          <t>58000</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>78000</t>
+        </is>
+      </c>
       <c r="F74" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2369,17 +2389,17 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Водитель на минивэн</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-31607317.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-na-miniven-30987950.html</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>100000</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
@@ -2395,17 +2415,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Начинающий специалист по обслуживанию клиентов</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32418797.html</t>
+          <t>http://www.superjob.ru/vakansii/nachinayuschij-specialist-po-obsluzhivaniyu-klientov-31670219.html</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>40000</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
@@ -2421,20 +2441,24 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Программист Delphi</t>
+          <t>Повар (м. Фрунзенская)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-delphi-32253244.html</t>
+          <t>http://www.superjob.ru/vakansii/povar-32268013.html</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>120000</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F77" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2447,17 +2471,17 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Программист 1С (Управление торговлей)</t>
+          <t>Продавец в супермаркет премиум-класса (Истринскй р-н, д. Покровское)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32294034.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-v-supermarket-premium-klassa-31128173.html</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>43000</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
@@ -2473,17 +2497,17 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Менеджер в минимаркет премиум-класса (м. Беговая, Университет, Выставочная, Деловой центр)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-28066679.html</t>
+          <t>http://www.superjob.ru/vakansii/menedzher-v-minimarket-premium-klassa-31160269.html</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>45000</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
@@ -2499,12 +2523,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Программист Bitrix</t>
+          <t>Мастер участка по ремонту кабельных линий 14 РЭР</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-bitrix-32518707.html</t>
+          <t>http://www.superjob.ru/vakansii/master-uchastka-po-remontu-kabelnyh-linij-14-rer-32330202.html</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2525,17 +2549,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Программист Full-stack</t>
+          <t>Риелтор по недвижимости</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-full-stack-32485752.html</t>
+          <t>http://www.superjob.ru/vakansii/rieltor-po-nedvizhimosti-32379651.html</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -2551,20 +2575,24 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Программист C#</t>
+          <t>Пекарь (м. Арбатская)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-c-32417721.html</t>
+          <t>http://www.superjob.ru/vakansii/pekar-32268014.html</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>110000</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F82" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2577,24 +2605,20 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Контролер на склад товаров для магазина</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32168465.html</t>
+          <t>http://www.superjob.ru/vakansii/kontroler-na-sklad-tovarov-dlya-magazina-32335576.html</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>80000</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>100000</t>
-        </is>
-      </c>
+          <t>Не указано</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2607,17 +2631,17 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Визитный мерчендайзер</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32442455.html</t>
+          <t>http://www.superjob.ru/vakansii/vizitnyj-merchendajzer-32335578.html</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>3900</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
@@ -2633,17 +2657,17 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Оператор по работе с клиентами</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-29964912.html</t>
+          <t>http://www.superjob.ru/vakansii/operator-po-rabote-s-klientami-32292362.html</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>150000</t>
+          <t>Не указано</t>
         </is>
       </c>
       <c r="E85" t="inlineStr"/>
@@ -2659,17 +2683,17 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32423853.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32292911.html</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>30000</t>
         </is>
       </c>
       <c r="E86" t="inlineStr"/>
@@ -2685,20 +2709,24 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Ведущий программист</t>
+          <t>Продавец-консультант (м. Новокосино, Новогиреево)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>/vakansii/veduschij-programmist-32480047.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-32392050.html</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>70000</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr"/>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>51000</t>
+        </is>
+      </c>
       <c r="F87" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2711,20 +2739,24 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Продавец-консультант</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32398952.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-31806604.html</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>200000</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr"/>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>95000</t>
+        </is>
+      </c>
       <c r="F88" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2737,17 +2769,17 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Программист</t>
+          <t>Старший повар</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-32508997.html</t>
+          <t>http://www.superjob.ru/vakansii/starshij-povar-32292909.html</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>70000</t>
+          <t>35000</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
@@ -2763,17 +2795,17 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Инженер-программист АСУ ТП</t>
+          <t>Директор магазина</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-asu-tp-32463972.html</t>
+          <t>http://www.superjob.ru/vakansii/direktor-magazina-32240008.html</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>100000</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
@@ -2789,20 +2821,24 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Педагог-психолог</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32415989.html</t>
+          <t>http://www.superjob.ru/vakansii/pedagog-psiholog-32116732.html</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Не указано</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr"/>
+          <t>48000</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
       <c r="F91" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2815,12 +2851,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Программист ABAP (специалист по разработке программ и интерфейсов)</t>
+          <t>Водитель такси категории Б</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-abap-31862231.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-taksi-kategorii-b-32454117.html</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2841,17 +2877,17 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Инженер-программист SQL</t>
+          <t>Медицинская сестра отделения вспомогательных репродуктивных технологий</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-sql-27841165.html</t>
+          <t>http://www.superjob.ru/vakansii/medicinskaya-sestra-otdeleniya-vspomogatelnyh-reproduktivnyh-tehnologij-32434455.html</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>52000</t>
+          <t>Не указано</t>
         </is>
       </c>
       <c r="E93" t="inlineStr"/>
@@ -2867,20 +2903,24 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Программист 1С</t>
+          <t>Продавец-консультант (ст. м. Фили)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-1s-32318409.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-konsultant-29970309.html</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>125000</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr"/>
+          <t>58000</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>78000</t>
+        </is>
+      </c>
       <c r="F94" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2893,17 +2933,17 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Программист</t>
+          <t>Водитель на минивэн</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-31802291.html</t>
+          <t>http://www.superjob.ru/vakansii/voditel-na-miniven-30987950.html</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Не указано</t>
+          <t>100000</t>
         </is>
       </c>
       <c r="E95" t="inlineStr"/>
@@ -2919,24 +2959,20 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Помощник программиста 1С</t>
+          <t>Начинающий специалист по обслуживанию клиентов</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>/vakansii/pomoschnik-programmista-1s-31315035.html</t>
+          <t>http://www.superjob.ru/vakansii/nachinayuschij-specialist-po-obsluzhivaniyu-klientov-31670219.html</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>17400</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>170000</t>
-        </is>
-      </c>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2949,20 +2985,24 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Программист</t>
+          <t>Повар (м. Фрунзенская)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-32403097.html</t>
+          <t>http://www.superjob.ru/vakansii/povar-32268013.html</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>100000</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr"/>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
       <c r="F97" t="inlineStr">
         <is>
           <t>SuperJob</t>
@@ -2975,17 +3015,17 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Инженер-программист станков с ЧПУ / Оператор-программист ЧПУ</t>
+          <t>Продавец в супермаркет премиум-класса (Истринскй р-н, д. Покровское)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>/vakansii/inzhener-programmist-stankov-s-chpu-32517168.html</t>
+          <t>http://www.superjob.ru/vakansii/prodavec-v-supermarket-premium-klassa-31128173.html</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>65000</t>
+          <t>43000</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
@@ -3001,17 +3041,17 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Программист C/С++</t>
+          <t>Менеджер в минимаркет премиум-класса (м. Беговая, Университет, Выставочная, Деловой центр)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-c-32118024.html</t>
+          <t>http://www.superjob.ru/vakansii/menedzher-v-minimarket-premium-klassa-31160269.html</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>120000</t>
+          <t>45000</t>
         </is>
       </c>
       <c r="E99" t="inlineStr"/>
@@ -3027,12 +3067,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Программист</t>
+          <t>Мастер участка по ремонту кабельных линий 14 РЭР</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>/vakansii/programmist-32396725.html</t>
+          <t>http://www.superjob.ru/vakansii/master-uchastka-po-remontu-kabelnyh-linij-14-rer-32330202.html</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3053,17 +3093,17 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Сервисный инженер 1С / Программист 1С</t>
+          <t>Риелтор по недвижимости</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>/vakansii/servisnyj-inzhener-1s-30191846.html</t>
+          <t>http://www.superjob.ru/vakansii/rieltor-po-nedvizhimosti-32379651.html</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>70000</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="E101" t="inlineStr"/>

</xml_diff>